<commit_message>
NER extraction models compare complete (Part 1) fix
</commit_message>
<xml_diff>
--- a/reports/research/05-research--ner_compare.xlsx
+++ b/reports/research/05-research--ner_compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jupyter\semantic_news_graph\reports\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF46D79F-F047-48B0-AD88-1BD097D07F93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F999E6DB-AE3F-4421-BE0A-B562A4410CC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="12">
   <si>
     <t>Accuracy (Full)</t>
   </si>
@@ -87,7 +87,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +97,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -128,13 +134,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +447,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +600,7 @@
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="4">
         <v>0.96793738127988471</v>
       </c>
       <c r="C7" s="2">
@@ -602,7 +609,7 @@
       <c r="D7" s="2">
         <v>30534</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="4">
         <v>0.96804746044962531</v>
       </c>
       <c r="F7" s="2">

</xml_diff>